<commit_message>
added clinical demographics table
</commit_message>
<xml_diff>
--- a/gantt chart spreadsheet.xlsx
+++ b/gantt chart spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florencetownend/Documents/Postgraduate/Upgrade/upgrade-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5683A60-2A2D-3D45-A1B7-C72C79D4995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB2EBED-9C31-9540-9610-CA03A6CCB314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D13FE16D-BADF-7644-A072-E894E4419087}"/>
+    <workbookView xWindow="30240" yWindow="-1260" windowWidth="38400" windowHeight="21600" xr2:uid="{D13FE16D-BADF-7644-A072-E894E4419087}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2B1CF-91C6-D14C-96AE-658C3B5E71F6}">
   <dimension ref="B4:W18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
written methods section of Cox models
</commit_message>
<xml_diff>
--- a/gantt chart spreadsheet.xlsx
+++ b/gantt chart spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florencetownend/Documents/Postgraduate/Upgrade/upgrade-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB2EBED-9C31-9540-9610-CA03A6CCB314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7F3A2B-FE0B-B44A-87C7-C7A22F73D3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1260" windowWidth="38400" windowHeight="21600" xr2:uid="{D13FE16D-BADF-7644-A072-E894E4419087}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{D13FE16D-BADF-7644-A072-E894E4419087}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,13 +95,13 @@
     <t>Project 3a: Prognosis definition sensitivity analysis</t>
   </si>
   <si>
-    <t>Project 1a: Fusilli with MND</t>
-  </si>
-  <si>
     <t>Project 1b: Fusilli with PPMI, ADNI, CXR</t>
   </si>
   <si>
     <t>Project 2: Effect of brain MRI preprocessing</t>
+  </si>
+  <si>
+    <t>Project 1a: Fusilli with MND - AND</t>
   </si>
 </sst>
 </file>
@@ -294,11 +294,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -306,20 +303,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -334,7 +321,7 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -343,7 +330,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2B1CF-91C6-D14C-96AE-658C3B5E71F6}">
-  <dimension ref="B4:W18"/>
+  <dimension ref="B4:W16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,353 +690,347 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:23" ht="27" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="29">
         <v>2024</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="11">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="30">
         <v>2025</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
     </row>
     <row r="5" spans="2:23" ht="22" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="32" t="s">
+      <c r="N5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="R5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="32" t="s">
+      <c r="S5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="32" t="s">
+      <c r="T5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
     </row>
     <row r="6" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="31"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="26"/>
     </row>
     <row r="7" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="26"/>
+    </row>
+    <row r="8" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="31"/>
-    </row>
-    <row r="8" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="26"/>
+    </row>
+    <row r="9" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="26"/>
+    </row>
+    <row r="10" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="31"/>
-    </row>
-    <row r="9" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="26"/>
+    </row>
+    <row r="11" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="31"/>
-    </row>
-    <row r="10" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B10" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="31"/>
-    </row>
-    <row r="11" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="26"/>
+    </row>
+    <row r="12" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="26"/>
+    </row>
+    <row r="13" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="26"/>
+    </row>
+    <row r="14" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="26"/>
+    </row>
+    <row r="15" spans="2:23" ht="19" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="31"/>
-    </row>
-    <row r="12" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="31"/>
-    </row>
-    <row r="13" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B13" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="31"/>
-    </row>
-    <row r="14" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="31"/>
-    </row>
-    <row r="15" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="31"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="26"/>
     </row>
     <row r="16" spans="2:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="22"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="9"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="9"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
altering future work and gantt chart
</commit_message>
<xml_diff>
--- a/gantt chart spreadsheet.xlsx
+++ b/gantt chart spreadsheet.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florencetownend/Documents/Postgraduate/Upgrade/upgrade-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7F3A2B-FE0B-B44A-87C7-C7A22F73D3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560C82F5-81BA-554B-8645-129AF21F4F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{D13FE16D-BADF-7644-A072-E894E4419087}"/>
+    <workbookView xWindow="33300" yWindow="1100" windowWidth="30240" windowHeight="18880" xr2:uid="{D13FE16D-BADF-7644-A072-E894E4419087}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$21:$U$30</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -102,13 +105,25 @@
   </si>
   <si>
     <t>Project 1a: Fusilli with MND - AND</t>
+  </si>
+  <si>
+    <t>Fusilli: Applying to other datasets and extending MND application</t>
+  </si>
+  <si>
+    <t>Final chapter options: prognosis definition sensitivity analysis or adding another data modality (spinal MRI or reports)</t>
+  </si>
+  <si>
+    <t>Effect of brain MRI preprocessing on multimodal prognosis prediction</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +160,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -206,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -290,11 +311,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -341,6 +391,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,16 +735,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD2B1CF-91C6-D14C-96AE-658C3B5E71F6}">
-  <dimension ref="B4:W16"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B4:W29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" customWidth="1"/>
     <col min="3" max="20" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1032,13 +1094,218 @@
       <c r="S16" s="16"/>
       <c r="T16" s="17"/>
     </row>
+    <row r="23" spans="2:21" ht="27" x14ac:dyDescent="0.2">
+      <c r="B23" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="29">
+        <v>2024</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="30">
+        <v>2025</v>
+      </c>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="9"/>
+    </row>
+    <row r="24" spans="2:21" ht="22" x14ac:dyDescent="0.2">
+      <c r="B24" s="29"/>
+      <c r="C24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="R24" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="S24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="U24" s="8"/>
+    </row>
+    <row r="25" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="26"/>
+    </row>
+    <row r="26" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="26"/>
+    </row>
+    <row r="27" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="26"/>
+    </row>
+    <row r="28" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="26"/>
+    </row>
+    <row r="29" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="L4:T4"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:K23"/>
+    <mergeCell ref="L23:T23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="63" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>